<commit_message>
Changed Template look and row numbers
</commit_message>
<xml_diff>
--- a/1 - CDP Switch Audit _ Template.xlsx
+++ b/1 - CDP Switch Audit _ Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP Network Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4963666d19cbf5d1/Documents/Network-Programmability/Pycharm Projects/CDP_Network_Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA5FDA0-C55D-45E5-9DB8-E67E84F34BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{AAA5FDA0-C55D-45E5-9DB8-E67E84F34BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E804A93-166B-4A5C-8414-BDDA3F7CD49D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Audit!$A$11:$I$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNS Resolved'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNS Resolved'!$A$4:$B$4</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>CDP Device Audit</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Connection Errors</t>
+  </si>
+  <si>
+    <t>DNS Resolved IP Addresses</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +128,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -205,6 +226,48 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,60 +613,60 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
-    <col min="8" max="8" width="120.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="50.6640625" customWidth="1"/>
+    <col min="8" max="8" width="120.6640625" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -645,70 +708,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}"/>
+  <autoFilter ref="A4:B4" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BC569B-A16A-4198-9DB5-FADCB4818C57}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C2847-EC79-480E-B4B3-31C0E0F06CAB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:2" s="24" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added folder for compiled zips
</commit_message>
<xml_diff>
--- a/1 - CDP Switch Audit _ Template.xlsx
+++ b/1 - CDP Switch Audit _ Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4963666d19cbf5d1/Documents/Network-Programmability/Pycharm Projects/CDP_Network_Map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDP Network Map V2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{AAA5FDA0-C55D-45E5-9DB8-E67E84F34BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E804A93-166B-4A5C-8414-BDDA3F7CD49D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F03D2-C9F0-4F6A-808F-30F127FB5943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,6 +215,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -230,44 +248,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,14 +622,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,15 +720,15 @@
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:2" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,20 +762,20 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:2" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +791,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,20 +799,20 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21"/>
-    </row>
-    <row r="2" spans="1:2" s="24" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>